<commit_message>
Cleaned Excel Sheet Updated
</commit_message>
<xml_diff>
--- a/Mini-Project/Cleaned_And_Formatted_Feedback.xlsx
+++ b/Mini-Project/Cleaned_And_Formatted_Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1496DD4-EE30-4C13-B062-BB6316AD24D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB112389-B849-4F8E-8E58-87E992DBA707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="157">
   <si>
     <t>Timestamp</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Education Background</t>
   </si>
 </sst>
 </file>
@@ -872,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X13"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,11 +888,15 @@
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="35.5546875" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,55 +922,61 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45899.948788032409</v>
       </c>
@@ -989,53 +1002,78 @@
       <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J2)),ISNUMBER(SEARCH("bscis",J2))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J2)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J2)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J2)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J2)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J2)),"BS Civil Engineering",
+J2))))))</f>
+        <v>BS Computer Science</v>
+      </c>
+      <c r="J2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("7",L2)),ISNUMBER(SEARCH("7th",L2))),"7th Semester",
+IF(OR(ISNUMBER(SEARCH("6",L2)),ISNUMBER(SEARCH("6th",L2))),"6th Semester",
+IF(OR(ISNUMBER(SEARCH("5",L2)),ISNUMBER(SEARCH("5th",L2))),"5th Semester",
+IF(OR(ISNUMBER(SEARCH("4",L2)),ISNUMBER(SEARCH("4th",L2))),"4th Semester",
+IF(OR(ISNUMBER(SEARCH("3",L2)),ISNUMBER(SEARCH("3rd",L2))),"3rd Semester",
+IF(OR(ISNUMBER(SEARCH("2",L2)),ISNUMBER(SEARCH("2nd",L2))),"2nd Semester",
+IF(OR(ISNUMBER(SEARCH("1st",L2)),""),"1st Semester",
+IF(ISNUMBER(SEARCH("final year",L2)),"Final Year",
+IF(ISNUMBER(SEARCH("graduate",L2)),"Fresh Graduate",
+IF(ISNUMBER(SEARCH("freelancer",L2)),"Freelancer",
+IF(ISNUMBER(SEARCH("engineer",L2)),"Civil Engineer",
+"Other")))))))))))</f>
+        <v>5th Semester</v>
+      </c>
+      <c r="L2" t="s">
         <v>67</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>77</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>79</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>81</v>
       </c>
-      <c r="N2" t="b">
+      <c r="P2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>93</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>100</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>102</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>114</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>78</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>127</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>138</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45899.948868414351</v>
       </c>
@@ -1061,47 +1099,72 @@
       <c r="H3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J3)),ISNUMBER(SEARCH("bscis",J3))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J3)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J3)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J3)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J3)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J3)),"BS Civil Engineering",
+J3))))))</f>
+        <v>BS Computer Science</v>
+      </c>
+      <c r="J3" t="s">
         <v>57</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K13" si="1">IF(OR(ISNUMBER(SEARCH("7",L3)),ISNUMBER(SEARCH("7th",L3))),"7th Semester",
+IF(OR(ISNUMBER(SEARCH("6",L3)),ISNUMBER(SEARCH("6th",L3))),"6th Semester",
+IF(OR(ISNUMBER(SEARCH("5",L3)),ISNUMBER(SEARCH("5th",L3))),"5th Semester",
+IF(OR(ISNUMBER(SEARCH("4",L3)),ISNUMBER(SEARCH("4th",L3))),"4th Semester",
+IF(OR(ISNUMBER(SEARCH("3",L3)),ISNUMBER(SEARCH("3rd",L3))),"3rd Semester",
+IF(OR(ISNUMBER(SEARCH("2",L3)),ISNUMBER(SEARCH("2nd",L3))),"2nd Semester",
+IF(OR(ISNUMBER(SEARCH("1st",L3)),""),"1st Semester",
+IF(ISNUMBER(SEARCH("final year",L3)),"Final Year",
+IF(ISNUMBER(SEARCH("graduate",L3)),"Fresh Graduate",
+IF(ISNUMBER(SEARCH("freelancer",L3)),"Freelancer",
+IF(ISNUMBER(SEARCH("engineer",L3)),"Civil Engineer",
+"Other")))))))))))</f>
+        <v>7th Semester</v>
+      </c>
+      <c r="L3" t="s">
         <v>68</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>77</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>80</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>82</v>
       </c>
-      <c r="N3" t="b">
+      <c r="P3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>94</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>98</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>101</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>103</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>115</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>126</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45899.951028321761</v>
       </c>
@@ -1127,53 +1190,67 @@
       <c r="H4" t="s">
         <v>51</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J4)),ISNUMBER(SEARCH("bscis",J4))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J4)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J4)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J4)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J4)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J4)),"BS Civil Engineering",
+J4))))))</f>
+        <v>BS Software Engineering</v>
+      </c>
+      <c r="J4" t="s">
         <v>58</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>7th Semester</v>
+      </c>
+      <c r="L4" t="s">
         <v>69</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>78</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>80</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>83</v>
       </c>
-      <c r="N4" t="b">
+      <c r="P4" t="b">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>93</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>97</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>101</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>104</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>116</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>78</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>129</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>139</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45899.955625752307</v>
       </c>
@@ -1199,47 +1276,61 @@
       <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J5)),ISNUMBER(SEARCH("bscis",J5))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J5)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J5)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J5)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J5)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J5)),"BS Civil Engineering",
+J5))))))</f>
+        <v>BS Software Engineering</v>
+      </c>
+      <c r="J5" t="s">
         <v>59</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>Freelancer</v>
+      </c>
+      <c r="L5" t="s">
         <v>70</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>78</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>80</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>84</v>
       </c>
-      <c r="N5" t="b">
+      <c r="P5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>95</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>97</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>100</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>105</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>117</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>77</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45899.962118761578</v>
       </c>
@@ -1265,53 +1356,67 @@
       <c r="H6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J6)),ISNUMBER(SEARCH("bscis",J6))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J6)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J6)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J6)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J6)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J6)),"BS Civil Engineering",
+J6))))))</f>
+        <v>BS Software Engineering</v>
+      </c>
+      <c r="J6" t="s">
         <v>58</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>Final Year</v>
+      </c>
+      <c r="L6" t="s">
         <v>71</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>78</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>80</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>85</v>
       </c>
-      <c r="N6" t="b">
+      <c r="P6" t="b">
         <v>1</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>93</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>97</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>100</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>106</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>118</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>78</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>130</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>140</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45899.963007835649</v>
       </c>
@@ -1337,53 +1442,67 @@
       <c r="H7" t="s">
         <v>53</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J7)),ISNUMBER(SEARCH("bscis",J7))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J7)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J7)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J7)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J7)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J7)),"BS Civil Engineering",
+J7))))))</f>
+        <v>BS Mathematics</v>
+      </c>
+      <c r="J7" t="s">
         <v>60</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>5th Semester</v>
+      </c>
+      <c r="L7" t="s">
         <v>72</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>78</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>80</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>86</v>
       </c>
-      <c r="N7" t="b">
+      <c r="P7" t="b">
         <v>1</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>94</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>100</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>107</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>119</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>78</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W7" t="s">
         <v>131</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>141</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45899.964712743058</v>
       </c>
@@ -1409,53 +1528,67 @@
       <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J8)),ISNUMBER(SEARCH("bscis",J8))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J8)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J8)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J8)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J8)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J8)),"BS Civil Engineering",
+J8))))))</f>
+        <v>BS Data Science</v>
+      </c>
+      <c r="J8" t="s">
         <v>61</v>
       </c>
-      <c r="J8">
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>4th Semester</v>
+      </c>
+      <c r="L8">
         <v>4</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>77</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>79</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>87</v>
       </c>
-      <c r="N8" t="b">
+      <c r="P8" t="b">
         <v>1</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>96</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>97</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>100</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>108</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>120</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>77</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
         <v>132</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>142</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Y8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45900.430683958337</v>
       </c>
@@ -1481,53 +1614,67 @@
       <c r="H9" t="s">
         <v>50</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J9)),ISNUMBER(SEARCH("bscis",J9))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J9)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J9)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J9)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J9)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J9)),"BS Civil Engineering",
+J9))))))</f>
+        <v>BS Computer Science</v>
+      </c>
+      <c r="J9" t="s">
         <v>62</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>5th Semester</v>
+      </c>
+      <c r="L9" t="s">
         <v>73</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>77</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>79</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>88</v>
       </c>
-      <c r="N9" t="b">
+      <c r="P9" t="b">
         <v>1</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>95</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>98</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>100</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>109</v>
       </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>121</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>78</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
         <v>133</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>143</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Y9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45900.44222863426</v>
       </c>
@@ -1553,53 +1700,67 @@
       <c r="H10" t="s">
         <v>52</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J10)),ISNUMBER(SEARCH("bscis",J10))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J10)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J10)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J10)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J10)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J10)),"BS Civil Engineering",
+J10))))))</f>
+        <v>BS Computer Engineering</v>
+      </c>
+      <c r="J10" t="s">
         <v>63</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>Fresh Graduate</v>
+      </c>
+      <c r="L10" t="s">
         <v>74</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>78</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>79</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>89</v>
       </c>
-      <c r="N10" t="b">
+      <c r="P10" t="b">
         <v>1</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>93</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>98</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>101</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>110</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>122</v>
       </c>
-      <c r="T10" t="s">
+      <c r="V10" t="s">
         <v>77</v>
       </c>
-      <c r="U10" t="s">
+      <c r="W10" t="s">
         <v>134</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>144</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Y10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45900.575352800923</v>
       </c>
@@ -1625,53 +1786,67 @@
       <c r="H11" t="s">
         <v>55</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J11)),ISNUMBER(SEARCH("bscis",J11))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J11)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J11)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J11)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J11)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J11)),"BS Civil Engineering",
+J11))))))</f>
+        <v>BS Civil Engineering</v>
+      </c>
+      <c r="J11" t="s">
         <v>64</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>Civil Engineer</v>
+      </c>
+      <c r="L11" t="s">
         <v>75</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>78</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>80</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>90</v>
       </c>
-      <c r="N11" t="b">
+      <c r="P11" t="b">
         <v>1</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>95</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>97</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>101</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>111</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>123</v>
       </c>
-      <c r="T11" t="s">
+      <c r="V11" t="s">
         <v>78</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" t="s">
         <v>135</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>145</v>
       </c>
-      <c r="W11" t="s">
+      <c r="Y11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45900.604983136567</v>
       </c>
@@ -1697,47 +1872,61 @@
       <c r="H12" t="s">
         <v>56</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J12)),ISNUMBER(SEARCH("bscis",J12))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J12)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J12)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J12)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J12)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J12)),"BS Civil Engineering",
+J12))))))</f>
+        <v>BS Data Science</v>
+      </c>
+      <c r="J12" t="s">
         <v>65</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>5th Semester</v>
+      </c>
+      <c r="L12" t="s">
         <v>67</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>77</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>80</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>91</v>
       </c>
-      <c r="N12" t="b">
+      <c r="P12" t="b">
         <v>1</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>95</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>98</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>100</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>112</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>124</v>
       </c>
-      <c r="T12" t="s">
+      <c r="V12" t="s">
         <v>77</v>
       </c>
-      <c r="U12" t="s">
+      <c r="W12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45900.721759189822</v>
       </c>
@@ -1763,43 +1952,57 @@
       <c r="H13" t="s">
         <v>50</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("computer science",J13)),ISNUMBER(SEARCH("bscis",J13))),"BS Computer Science",
+IF(ISNUMBER(SEARCH("software engineering",J13)),"BS Software Engineering",
+IF(ISNUMBER(SEARCH("mathematics",J13)),"BS Mathematics",
+IF(ISNUMBER(SEARCH("data science",J13)),"BS Data Science",
+IF(ISNUMBER(SEARCH("computer engineering",J13)),"BS Computer Engineering",
+IF(ISNUMBER(SEARCH("civil engineering",J13)),"BS Civil Engineering",
+J13))))))</f>
+        <v>BS Data Science</v>
+      </c>
+      <c r="J13" t="s">
         <v>66</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>3rd Semester</v>
+      </c>
+      <c r="L13" t="s">
         <v>76</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>77</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>79</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>92</v>
       </c>
-      <c r="N13" t="b">
+      <c r="P13" t="b">
         <v>1</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>95</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>98</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>101</v>
       </c>
-      <c r="R13" t="s">
+      <c r="T13" t="s">
         <v>113</v>
       </c>
-      <c r="S13" t="s">
+      <c r="U13" t="s">
         <v>125</v>
       </c>
-      <c r="T13" t="s">
+      <c r="V13" t="s">
         <v>77</v>
       </c>
-      <c r="U13" t="s">
+      <c r="W13" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Excel Sheet & Dashboard
</commit_message>
<xml_diff>
--- a/Mini-Project/Cleaned_And_Formatted_Feedback.xlsx
+++ b/Mini-Project/Cleaned_And_Formatted_Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB112389-B849-4F8E-8E58-87E992DBA707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2206A943-FB3A-45E3-AF99-9624CB5DF639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="162">
   <si>
     <t>Timestamp</t>
   </si>
@@ -504,6 +504,21 @@
   </si>
   <si>
     <t>Education Background</t>
+  </si>
+  <si>
+    <t>Suggestions</t>
+  </si>
+  <si>
+    <t>Takeways</t>
+  </si>
+  <si>
+    <t>Messaging Peers</t>
+  </si>
+  <si>
+    <t>Weekly Actions Summary</t>
+  </si>
+  <si>
+    <t>Support Needed Summary</t>
   </si>
 </sst>
 </file>
@@ -875,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,9 +909,17 @@
     <col min="11" max="11" width="13.109375" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.6640625" customWidth="1"/>
+    <col min="20" max="20" width="51.44140625" customWidth="1"/>
+    <col min="21" max="22" width="117.6640625" customWidth="1"/>
+    <col min="23" max="23" width="83.33203125" customWidth="1"/>
+    <col min="24" max="25" width="31.6640625" customWidth="1"/>
+    <col min="26" max="27" width="87.77734375" customWidth="1"/>
+    <col min="28" max="29" width="86.6640625" customWidth="1"/>
+    <col min="30" max="30" width="194.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,28 +978,40 @@
         <v>14</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45899.948788032409</v>
       </c>
@@ -1003,7 +1038,7 @@
         <v>50</v>
       </c>
       <c r="I2" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J2)),ISNUMBER(SEARCH("bscis",J2))),"BS Computer Science",
+        <f t="shared" ref="I2:I13" si="0">IF(OR(ISNUMBER(SEARCH("computer science",J2)),ISNUMBER(SEARCH("bscis",J2))),"BS Computer Science",
 IF(ISNUMBER(SEARCH("software engineering",J2)),"BS Software Engineering",
 IF(ISNUMBER(SEARCH("mathematics",J2)),"BS Mathematics",
 IF(ISNUMBER(SEARCH("data science",J2)),"BS Data Science",
@@ -1054,26 +1089,69 @@
       <c r="S2" t="s">
         <v>100</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" t="str">
+        <f>IF(ISNUMBER(SEARCH("daily",U2)),"Consistency",
+ IF(ISNUMBER(SEARCH("learn",U2)),"Learning",
+ IF(ISNUMBER(SEARCH("community",U2)),"Community",
+ IF(ISNUMBER(SEARCH("time",U2)),"Time Mgmt","Other"))))</f>
+        <v>Other</v>
+      </c>
+      <c r="U2" t="s">
         <v>102</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="str">
+        <f>IF(ISNUMBER(SEARCH("guide",W2)),"Guidance",
+ IF(ISNUMBER(SEARCH("peer",W2)),"Community",
+ IF(ISNUMBER(SEARCH("network",W2)),"Community",
+ IF(ISNUMBER(SEARCH("reminder",W2)),"Motivation",
+ IF(ISNUMBER(SEARCH("internet",W2)),"Resources","Other")))))</f>
+        <v>Other</v>
+      </c>
+      <c r="W2" t="s">
         <v>114</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>78</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="str">
+        <f>IF(OR(ISNUMBER(SEARCH("clear",Z2)),ISNUMBER(SEARCH("guid",Z2)),ISNUMBER(SEARCH("explain",Z2))),"Clarity",
+ IF(OR(ISNUMBER(SEARCH("project",Z2)),ISNUMBER(SEARCH("practical",Z2)),ISNUMBER(SEARCH("hands",Z2)),ISNUMBER(SEARCH("exercise",Z2))),"Hands-on",
+ IF(OR(ISNUMBER(SEARCH("deadline",Z2)),ISNUMBER(SEARCH("weekly",Z2)),ISNUMBER(SEARCH("daily",Z2)),ISNUMBER(SEARCH("time",Z2))),"Flexibility",
+ IF(OR(ISNUMBER(SEARCH("peer",Z2)),ISNUMBER(SEARCH("collaborat",Z2)),ISNUMBER(SEARCH("group",Z2)),ISNUMBER(SEARCH("team",Z2))),"Engagement",
+ IF(OR(ISNUMBER(SEARCH("speed",Z2)),ISNUMBER(SEARCH("fast",Z2)),ISNUMBER(SEARCH("slow",Z2))),"Pacing",
+ IF(OR(ISNUMBER(SEARCH("resource",Z2)),ISNUMBER(SEARCH("material",Z2)),ISNUMBER(SEARCH("slide",Z2)),ISNUMBER(SEARCH("doc",Z2))),"Resources",
+ IF(OR(ISNUMBER(SEARCH("facilitator",Z2)),ISNUMBER(SEARCH("mentor",Z2)),ISNUMBER(SEARCH("teacher",Z2))),"Facilitation",
+ IF(ISNUMBER(SEARCH("no comment",Z2)),"Nothing","Other"))))))))</f>
+        <v>Other</v>
+      </c>
+      <c r="Z2" t="s">
         <v>127</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="str">
+        <f>IFERROR(
+   IF(ISNUMBER(SEARCH("consist",AB2)),"Consistency",
+   IF(ISNUMBER(SEARCH("growth",AB2)),"Growth",
+   IF(ISNUMBER(SEARCH("focus",AB2)),"Focus",
+   IF(ISNUMBER(SEARCH("time",AB2)),"Focus",
+   "Motivation")))),
+"Motivation")</f>
+        <v>Motivation</v>
+      </c>
+      <c r="AB2" t="s">
         <v>138</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AC2" t="str">
+        <f>IF(ISNUMBER(SEARCH("collaborate",AD2)),"Collaboration",
+ IF(ISNUMBER(SEARCH("push",AD2)),"Motivation",
+ IF(ISNUMBER(SEARCH("learn",AD2)),"Learning",
+ IF(OR(AD2="",AD2="No"),"None","Other"))))</f>
+        <v>Other</v>
+      </c>
+      <c r="AD2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45899.948868414351</v>
       </c>
@@ -1081,7 +1159,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C13" si="0">LOWER(D3)</f>
+        <f t="shared" ref="C3:C13" si="1">LOWER(D3)</f>
         <v>muhibajaz333@gmail.com</v>
       </c>
       <c r="D3" t="s">
@@ -1100,20 +1178,14 @@
         <v>50</v>
       </c>
       <c r="I3" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J3)),ISNUMBER(SEARCH("bscis",J3))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J3)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J3)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J3)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J3)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J3)),"BS Civil Engineering",
-J3))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Computer Science</v>
       </c>
       <c r="J3" t="s">
         <v>57</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K13" si="1">IF(OR(ISNUMBER(SEARCH("7",L3)),ISNUMBER(SEARCH("7th",L3))),"7th Semester",
+        <f t="shared" ref="K3:K13" si="2">IF(OR(ISNUMBER(SEARCH("7",L3)),ISNUMBER(SEARCH("7th",L3))),"7th Semester",
 IF(OR(ISNUMBER(SEARCH("6",L3)),ISNUMBER(SEARCH("6th",L3))),"6th Semester",
 IF(OR(ISNUMBER(SEARCH("5",L3)),ISNUMBER(SEARCH("5th",L3))),"5th Semester",
 IF(OR(ISNUMBER(SEARCH("4",L3)),ISNUMBER(SEARCH("4th",L3))),"4th Semester",
@@ -1151,20 +1223,63 @@
       <c r="S3" t="s">
         <v>101</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T13" si="3">IF(ISNUMBER(SEARCH("daily",U3)),"Consistency",
+ IF(ISNUMBER(SEARCH("learn",U3)),"Learning",
+ IF(ISNUMBER(SEARCH("community",U3)),"Community",
+ IF(ISNUMBER(SEARCH("time",U3)),"Time Mgmt","Other"))))</f>
+        <v>Consistency</v>
+      </c>
+      <c r="U3" t="s">
         <v>103</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V13" si="4">IF(ISNUMBER(SEARCH("guide",W3)),"Guidance",
+ IF(ISNUMBER(SEARCH("peer",W3)),"Community",
+ IF(ISNUMBER(SEARCH("network",W3)),"Community",
+ IF(ISNUMBER(SEARCH("reminder",W3)),"Motivation",
+ IF(ISNUMBER(SEARCH("internet",W3)),"Resources","Other")))))</f>
+        <v>Community</v>
+      </c>
+      <c r="W3" t="s">
         <v>115</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>126</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="str">
+        <f t="shared" ref="Y3:Y13" si="5">IF(OR(ISNUMBER(SEARCH("clear",Z3)),ISNUMBER(SEARCH("guid",Z3)),ISNUMBER(SEARCH("explain",Z3))),"Clarity",
+ IF(OR(ISNUMBER(SEARCH("project",Z3)),ISNUMBER(SEARCH("practical",Z3)),ISNUMBER(SEARCH("hands",Z3)),ISNUMBER(SEARCH("exercise",Z3))),"Hands-on",
+ IF(OR(ISNUMBER(SEARCH("deadline",Z3)),ISNUMBER(SEARCH("weekly",Z3)),ISNUMBER(SEARCH("daily",Z3)),ISNUMBER(SEARCH("time",Z3))),"Flexibility",
+ IF(OR(ISNUMBER(SEARCH("peer",Z3)),ISNUMBER(SEARCH("collaborat",Z3)),ISNUMBER(SEARCH("group",Z3)),ISNUMBER(SEARCH("team",Z3))),"Engagement",
+ IF(OR(ISNUMBER(SEARCH("speed",Z3)),ISNUMBER(SEARCH("fast",Z3)),ISNUMBER(SEARCH("slow",Z3))),"Pacing",
+ IF(OR(ISNUMBER(SEARCH("resource",Z3)),ISNUMBER(SEARCH("material",Z3)),ISNUMBER(SEARCH("slide",Z3)),ISNUMBER(SEARCH("doc",Z3))),"Resources",
+ IF(OR(ISNUMBER(SEARCH("facilitator",Z3)),ISNUMBER(SEARCH("mentor",Z3)),ISNUMBER(SEARCH("teacher",Z3))),"Facilitation",
+ IF(ISNUMBER(SEARCH("no comment",Z3)),"Nothing","Other"))))))))</f>
+        <v>Nothing</v>
+      </c>
+      <c r="Z3" t="s">
         <v>128</v>
       </c>
+      <c r="AA3" t="str">
+        <f t="shared" ref="AA3:AA13" si="6">IFERROR(
+   IF(ISNUMBER(SEARCH("consist",AB3)),"Consistency",
+   IF(ISNUMBER(SEARCH("growth",AB3)),"Growth",
+   IF(ISNUMBER(SEARCH("focus",AB3)),"Focus",
+   IF(ISNUMBER(SEARCH("time",AB3)),"Focus",
+   "Motivation")))),
+"Motivation")</f>
+        <v>Motivation</v>
+      </c>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC12" si="7">IF(ISNUMBER(SEARCH("collaborate",AD3)),"Collaboration",
+ IF(ISNUMBER(SEARCH("push",AD3)),"Motivation",
+ IF(ISNUMBER(SEARCH("learn",AD3)),"Learning",
+ IF(OR(AD3="",AD3="No"),"None","Other"))))</f>
+        <v>None</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45899.951028321761</v>
       </c>
@@ -1172,7 +1287,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>mahmadshafi861@gmail.com</v>
       </c>
       <c r="D4" t="s">
@@ -1191,20 +1306,14 @@
         <v>51</v>
       </c>
       <c r="I4" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J4)),ISNUMBER(SEARCH("bscis",J4))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J4)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J4)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J4)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J4)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J4)),"BS Civil Engineering",
-J4))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Software Engineering</v>
       </c>
       <c r="J4" t="s">
         <v>58</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7th Semester</v>
       </c>
       <c r="L4" t="s">
@@ -1231,26 +1340,46 @@
       <c r="S4" t="s">
         <v>101</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" t="str">
+        <f t="shared" si="3"/>
+        <v>Learning</v>
+      </c>
+      <c r="U4" t="s">
         <v>104</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W4" t="s">
         <v>116</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>78</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="str">
+        <f t="shared" si="5"/>
+        <v>Flexibility</v>
+      </c>
+      <c r="Z4" t="s">
         <v>129</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AA4" t="str">
+        <f t="shared" si="6"/>
+        <v>Consistency</v>
+      </c>
+      <c r="AB4" t="s">
         <v>139</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AC4" t="str">
+        <f t="shared" si="7"/>
+        <v>Collaboration</v>
+      </c>
+      <c r="AD4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45899.955625752307</v>
       </c>
@@ -1258,7 +1387,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ahmedhassan5291520@gmail.com</v>
       </c>
       <c r="D5" t="s">
@@ -1277,20 +1406,14 @@
         <v>52</v>
       </c>
       <c r="I5" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J5)),ISNUMBER(SEARCH("bscis",J5))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J5)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J5)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J5)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J5)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J5)),"BS Civil Engineering",
-J5))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Software Engineering</v>
       </c>
       <c r="J5" t="s">
         <v>59</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Freelancer</v>
       </c>
       <c r="L5" t="s">
@@ -1317,20 +1440,40 @@
       <c r="S5" t="s">
         <v>100</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" t="str">
+        <f t="shared" si="3"/>
+        <v>Learning</v>
+      </c>
+      <c r="U5" t="s">
         <v>105</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W5" t="s">
         <v>117</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>77</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Y5" t="str">
+        <f t="shared" si="5"/>
+        <v>Other</v>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AC5" t="str">
+        <f t="shared" si="7"/>
+        <v>Other</v>
+      </c>
+      <c r="AD5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45899.962118761578</v>
       </c>
@@ -1338,7 +1481,7 @@
         <v>26</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>mohsinaleem680@gmail.com</v>
       </c>
       <c r="D6" t="s">
@@ -1357,20 +1500,14 @@
         <v>50</v>
       </c>
       <c r="I6" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J6)),ISNUMBER(SEARCH("bscis",J6))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J6)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J6)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J6)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J6)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J6)),"BS Civil Engineering",
-J6))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Software Engineering</v>
       </c>
       <c r="J6" t="s">
         <v>58</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Final Year</v>
       </c>
       <c r="L6" t="s">
@@ -1397,26 +1534,46 @@
       <c r="S6" t="s">
         <v>100</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" t="str">
+        <f t="shared" si="3"/>
+        <v>Other</v>
+      </c>
+      <c r="U6" t="s">
         <v>106</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W6" t="s">
         <v>118</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>78</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="str">
+        <f t="shared" si="5"/>
+        <v>Hands-on</v>
+      </c>
+      <c r="Z6" t="s">
         <v>130</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AA6" t="str">
+        <f t="shared" si="6"/>
+        <v>Growth</v>
+      </c>
+      <c r="AB6" t="s">
         <v>140</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AC6" t="str">
+        <f t="shared" si="7"/>
+        <v>Learning</v>
+      </c>
+      <c r="AD6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45899.963007835649</v>
       </c>
@@ -1424,7 +1581,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>uneebashaikh33@gmail.com</v>
       </c>
       <c r="D7" t="s">
@@ -1443,20 +1600,14 @@
         <v>53</v>
       </c>
       <c r="I7" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J7)),ISNUMBER(SEARCH("bscis",J7))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J7)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J7)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J7)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J7)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J7)),"BS Civil Engineering",
-J7))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Mathematics</v>
       </c>
       <c r="J7" t="s">
         <v>60</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5th Semester</v>
       </c>
       <c r="L7" t="s">
@@ -1483,26 +1634,46 @@
       <c r="S7" t="s">
         <v>100</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" t="str">
+        <f t="shared" si="3"/>
+        <v>Learning</v>
+      </c>
+      <c r="U7" t="s">
         <v>107</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W7" t="s">
         <v>119</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>78</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="str">
+        <f t="shared" si="5"/>
+        <v>Clarity</v>
+      </c>
+      <c r="Z7" t="s">
         <v>131</v>
       </c>
-      <c r="X7" t="s">
+      <c r="AA7" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AB7" t="s">
         <v>141</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AC7" t="str">
+        <f t="shared" si="7"/>
+        <v>None</v>
+      </c>
+      <c r="AD7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45899.964712743058</v>
       </c>
@@ -1510,7 +1681,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ahsanatiq789@gmail.com</v>
       </c>
       <c r="D8" t="s">
@@ -1529,20 +1700,14 @@
         <v>54</v>
       </c>
       <c r="I8" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J8)),ISNUMBER(SEARCH("bscis",J8))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J8)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J8)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J8)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J8)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J8)),"BS Civil Engineering",
-J8))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Data Science</v>
       </c>
       <c r="J8" t="s">
         <v>61</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4th Semester</v>
       </c>
       <c r="L8">
@@ -1569,26 +1734,46 @@
       <c r="S8" t="s">
         <v>100</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" t="str">
+        <f t="shared" si="3"/>
+        <v>Learning</v>
+      </c>
+      <c r="U8" t="s">
         <v>108</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W8" t="s">
         <v>120</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>77</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Y8" t="str">
+        <f t="shared" si="5"/>
+        <v>Flexibility</v>
+      </c>
+      <c r="Z8" t="s">
         <v>132</v>
       </c>
-      <c r="X8" t="s">
+      <c r="AA8" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AB8" t="s">
         <v>142</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AC8" t="str">
+        <f t="shared" si="7"/>
+        <v>Other</v>
+      </c>
+      <c r="AD8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45900.430683958337</v>
       </c>
@@ -1596,7 +1781,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>darainhyder21@gmail.com</v>
       </c>
       <c r="D9" t="s">
@@ -1615,20 +1800,14 @@
         <v>50</v>
       </c>
       <c r="I9" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J9)),ISNUMBER(SEARCH("bscis",J9))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J9)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J9)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J9)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J9)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J9)),"BS Civil Engineering",
-J9))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Computer Science</v>
       </c>
       <c r="J9" t="s">
         <v>62</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5th Semester</v>
       </c>
       <c r="L9" t="s">
@@ -1655,26 +1834,46 @@
       <c r="S9" t="s">
         <v>100</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" t="str">
+        <f t="shared" si="3"/>
+        <v>Other</v>
+      </c>
+      <c r="U9" t="s">
         <v>109</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="str">
+        <f t="shared" si="4"/>
+        <v>Resources</v>
+      </c>
+      <c r="W9" t="s">
         <v>121</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>78</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Y9" t="str">
+        <f t="shared" si="5"/>
+        <v>Other</v>
+      </c>
+      <c r="Z9" t="s">
         <v>133</v>
       </c>
-      <c r="X9" t="s">
+      <c r="AA9" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AB9" t="s">
         <v>143</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AC9" t="str">
+        <f t="shared" si="7"/>
+        <v>Other</v>
+      </c>
+      <c r="AD9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45900.44222863426</v>
       </c>
@@ -1682,7 +1881,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>myself.abdullahasif@gmail.com</v>
       </c>
       <c r="D10" t="s">
@@ -1701,20 +1900,14 @@
         <v>52</v>
       </c>
       <c r="I10" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J10)),ISNUMBER(SEARCH("bscis",J10))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J10)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J10)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J10)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J10)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J10)),"BS Civil Engineering",
-J10))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Computer Engineering</v>
       </c>
       <c r="J10" t="s">
         <v>63</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Fresh Graduate</v>
       </c>
       <c r="L10" t="s">
@@ -1741,26 +1934,46 @@
       <c r="S10" t="s">
         <v>101</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" t="str">
+        <f t="shared" si="3"/>
+        <v>Other</v>
+      </c>
+      <c r="U10" t="s">
         <v>110</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="str">
+        <f t="shared" si="4"/>
+        <v>Guidance</v>
+      </c>
+      <c r="W10" t="s">
         <v>122</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>77</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Y10" t="str">
+        <f t="shared" si="5"/>
+        <v>Other</v>
+      </c>
+      <c r="Z10" t="s">
         <v>134</v>
       </c>
-      <c r="X10" t="s">
+      <c r="AA10" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AB10" t="s">
         <v>144</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AC10" t="str">
+        <f t="shared" si="7"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AD10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45900.575352800923</v>
       </c>
@@ -1768,7 +1981,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>saliu.abdulazeezp@gmail.com</v>
       </c>
       <c r="D11" t="s">
@@ -1787,20 +2000,14 @@
         <v>55</v>
       </c>
       <c r="I11" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J11)),ISNUMBER(SEARCH("bscis",J11))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J11)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J11)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J11)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J11)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J11)),"BS Civil Engineering",
-J11))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Civil Engineering</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Civil Engineer</v>
       </c>
       <c r="L11" t="s">
@@ -1827,26 +2034,46 @@
       <c r="S11" t="s">
         <v>101</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" t="str">
+        <f t="shared" si="3"/>
+        <v>Other</v>
+      </c>
+      <c r="U11" t="s">
         <v>111</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W11" t="s">
         <v>123</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>78</v>
       </c>
-      <c r="W11" t="s">
+      <c r="Y11" t="str">
+        <f t="shared" si="5"/>
+        <v>Flexibility</v>
+      </c>
+      <c r="Z11" t="s">
         <v>135</v>
       </c>
-      <c r="X11" t="s">
+      <c r="AA11" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AB11" t="s">
         <v>145</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AC11" t="str">
+        <f t="shared" si="7"/>
+        <v>Other</v>
+      </c>
+      <c r="AD11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45900.604983136567</v>
       </c>
@@ -1854,7 +2081,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>sheikhanastauseef@gmail.com</v>
       </c>
       <c r="D12" t="s">
@@ -1873,20 +2100,14 @@
         <v>56</v>
       </c>
       <c r="I12" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J12)),ISNUMBER(SEARCH("bscis",J12))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J12)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J12)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J12)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J12)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J12)),"BS Civil Engineering",
-J12))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Data Science</v>
       </c>
       <c r="J12" t="s">
         <v>65</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5th Semester</v>
       </c>
       <c r="L12" t="s">
@@ -1913,20 +2134,40 @@
       <c r="S12" t="s">
         <v>100</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" t="str">
+        <f t="shared" si="3"/>
+        <v>Other</v>
+      </c>
+      <c r="U12" t="s">
         <v>112</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="str">
+        <f t="shared" si="4"/>
+        <v>Motivation</v>
+      </c>
+      <c r="W12" t="s">
         <v>124</v>
       </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
         <v>77</v>
       </c>
-      <c r="W12" t="s">
+      <c r="Y12" t="str">
+        <f t="shared" si="5"/>
+        <v>Flexibility</v>
+      </c>
+      <c r="Z12" t="s">
         <v>136</v>
       </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
+      </c>
+      <c r="AC12" t="str">
+        <f t="shared" si="7"/>
+        <v>None</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45900.721759189822</v>
       </c>
@@ -1934,7 +2175,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>m.a.h.works17@gmail.com</v>
       </c>
       <c r="D13" t="s">
@@ -1953,20 +2194,14 @@
         <v>50</v>
       </c>
       <c r="I13" t="str">
-        <f>IF(OR(ISNUMBER(SEARCH("computer science",J13)),ISNUMBER(SEARCH("bscis",J13))),"BS Computer Science",
-IF(ISNUMBER(SEARCH("software engineering",J13)),"BS Software Engineering",
-IF(ISNUMBER(SEARCH("mathematics",J13)),"BS Mathematics",
-IF(ISNUMBER(SEARCH("data science",J13)),"BS Data Science",
-IF(ISNUMBER(SEARCH("computer engineering",J13)),"BS Computer Engineering",
-IF(ISNUMBER(SEARCH("civil engineering",J13)),"BS Civil Engineering",
-J13))))))</f>
+        <f t="shared" si="0"/>
         <v>BS Data Science</v>
       </c>
       <c r="J13" t="s">
         <v>66</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3rd Semester</v>
       </c>
       <c r="L13" t="s">
@@ -1993,17 +2228,33 @@
       <c r="S13" t="s">
         <v>101</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" t="str">
+        <f t="shared" si="3"/>
+        <v>Learning</v>
+      </c>
+      <c r="U13" t="s">
         <v>113</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="str">
+        <f t="shared" si="4"/>
+        <v>Other</v>
+      </c>
+      <c r="W13" t="s">
         <v>125</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
         <v>77</v>
       </c>
-      <c r="W13" t="s">
+      <c r="Y13" t="str">
+        <f t="shared" si="5"/>
+        <v>Other</v>
+      </c>
+      <c r="Z13" t="s">
         <v>137</v>
+      </c>
+      <c r="AA13" t="str">
+        <f t="shared" si="6"/>
+        <v>Motivation</v>
       </c>
     </row>
   </sheetData>

</xml_diff>